<commit_message>
update french lakes' simulation
</commit_message>
<xml_diff>
--- a/data/model-population-parameters.xlsx
+++ b/data/model-population-parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91D4DFA-62DC-8347-925F-9016DA2A735F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7DCEBD-BA80-474C-91A9-E2DC960A081D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29180" windowHeight="17560" xr2:uid="{0419B776-088C-7F40-B532-C37DCE4D60FB}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +560,7 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
@@ -592,7 +592,7 @@
         <v>13</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
@@ -618,7 +618,7 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
update heatmaps and add workflow diagram
</commit_message>
<xml_diff>
--- a/data/model-population-parameters.xlsx
+++ b/data/model-population-parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7DCEBD-BA80-474C-91A9-E2DC960A081D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF39FBAE-21BA-2040-A7AE-4F3774D63BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29180" windowHeight="17560" xr2:uid="{0419B776-088C-7F40-B532-C37DCE4D60FB}"/>
   </bookViews>
@@ -153,8 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +473,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,8 +482,8 @@
     <col min="2" max="3" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -510,10 +511,10 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -565,10 +566,10 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>8.0749999999999993</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>6.5250000000000004</v>
       </c>
     </row>
@@ -724,10 +725,10 @@
       <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>4.1163189999999998</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>2.6932369999999999</v>
       </c>
     </row>
@@ -756,10 +757,10 @@
       <c r="H10" t="s">
         <v>17</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>4.3053720000000002</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>3.0243989999999998</v>
       </c>
     </row>
@@ -788,10 +789,10 @@
       <c r="H11" t="s">
         <v>17</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>5.4416669999999998</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>4.7750000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update TB temp data
</commit_message>
<xml_diff>
--- a/data/model-population-parameters.xlsx
+++ b/data/model-population-parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F860D5F4-4055-DF44-9867-33475FFCD51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3713BFE-2A8F-654D-9ABB-4A66C04F5E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29180" windowHeight="17560" xr2:uid="{0419B776-088C-7F40-B532-C37DCE4D60FB}"/>
+    <workbookView xWindow="13040" yWindow="500" windowWidth="20560" windowHeight="17560" xr2:uid="{0419B776-088C-7F40-B532-C37DCE4D60FB}"/>
   </bookViews>
   <sheets>
     <sheet name="bio-parameters" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,10 +808,10 @@
         <v>8</v>
       </c>
       <c r="I11" s="1">
-        <v>5.4416669999999998</v>
+        <v>4.943492</v>
       </c>
       <c r="J11" s="1">
-        <v>4.7750000000000004</v>
+        <v>4.3679399999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add chaumont bay NOAA temps
</commit_message>
<xml_diff>
--- a/data/model-population-parameters.xlsx
+++ b/data/model-population-parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3713BFE-2A8F-654D-9ABB-4A66C04F5E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5528B0B5-D5A5-D145-A6DF-BA325A52A3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="500" windowWidth="20560" windowHeight="17560" xr2:uid="{0419B776-088C-7F40-B532-C37DCE4D60FB}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add slope comp figure
</commit_message>
<xml_diff>
--- a/data/model-population-parameters.xlsx
+++ b/data/model-population-parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA721B3-309A-B24F-A652-081EA35270AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829E3D4B-70D4-E747-BF6F-D5A350878428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="500" windowWidth="20560" windowHeight="17560" xr2:uid="{0419B776-088C-7F40-B532-C37DCE4D60FB}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,6 +697,12 @@
       <c r="H7" t="s">
         <v>6</v>
       </c>
+      <c r="I7" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>